<commit_message>
Changes in calculation files
</commit_message>
<xml_diff>
--- a/Data/Trial Data/PowerWorldFormat.xlsx
+++ b/Data/Trial Data/PowerWorldFormat.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="100">
   <si>
     <t>Interface Name</t>
   </si>
@@ -34,19 +34,10 @@
     <t>Monitored Element Name</t>
   </si>
   <si>
-    <t>L_CIBOLO8_1Y-L_SCHERT8_1Y FLO HILLCTY_-L_MARION</t>
-  </si>
-  <si>
-    <t>TNCADDO___1-TNAPACHE__1 FLO TNTEJAS-TNGRENB</t>
-  </si>
-  <si>
-    <t>SONR4A-CAUTHORN4A FLO L_ODLASW-L_BLEWE</t>
-  </si>
-  <si>
-    <t>BALLINGE2A-BALEXTP2 FLO BALLINGE-COLE_IVI</t>
-  </si>
-  <si>
-    <t>RINCON4A-WHITEPT4A FLO HECKER4A-WHITEPT4</t>
+    <t>ASHERTON4A-CATARINA4 FLO MIGUEL5-LOBO7A</t>
+  </si>
+  <si>
+    <t>L_WIRTZ_8_1Y-L_FLATRO8_1Y FLO L_WIRTZ_-L_STARCK</t>
   </si>
   <si>
     <t>BALEXTP2-NOVC2A FLO BALLINGE-COLE_IVI</t>
@@ -55,196 +46,274 @@
     <t>GRESHRD_8-NACPW_1_8 FLO BASE</t>
   </si>
   <si>
-    <t>FTST4A-SOLSTICE4A FLO LINTERN-REROCK</t>
-  </si>
-  <si>
-    <t>HAMILTON4B-MAXWELL4A FLO ASHERTON-L_BEVO_</t>
-  </si>
-  <si>
-    <t>FALCON8-FALCONSW4A FLO FALCON8-FALCONS</t>
-  </si>
-  <si>
-    <t>SO_TEX__345A-DOW____POI_5 FLO W_A_P__-HILLJE_</t>
-  </si>
-  <si>
-    <t>ALPINE2A-BRONCO2A FLO FTST2A-COCS2A</t>
-  </si>
-  <si>
-    <t>CELANEBI4A-N_SHARPE4C FLO B_DAVIS4-ALAZAN4A</t>
-  </si>
-  <si>
-    <t>HAMILTON4A-MAVERICK4A FLO ASHERTON-L_BEVO_</t>
-  </si>
-  <si>
-    <t>MCNEILN-HOWARDLN FLO DUNLAP8-DECK_MB3</t>
-  </si>
-  <si>
-    <t>BRANCH 7608 7610 1</t>
-  </si>
-  <si>
-    <t>BRANCHOPEN 5211 7044 1</t>
-  </si>
-  <si>
-    <t>BRANCH 38710 38720 1</t>
-  </si>
-  <si>
-    <t>BRANCHOPEN 38530 38575 1</t>
-  </si>
-  <si>
-    <t>BRANCH 6515 8259 1</t>
-  </si>
-  <si>
-    <t>BRANCHOPEN 7425 78424 1</t>
-  </si>
-  <si>
-    <t>BRANCH 6338 6341 1</t>
+    <t>FRPHILLT2A-L_GILLES9_1Y FLO YELWJCKT-L_FORTM</t>
+  </si>
+  <si>
+    <t>TRUMBULL8-ENNSSW_8 FLO ENNS_W_8-WAX_8</t>
+  </si>
+  <si>
+    <t>RINCON4A-WHITEPT4A FLO PORTLAND-MCCAMPB</t>
+  </si>
+  <si>
+    <t>DOLRHIDE_8-NOTSW_1_8 FLO MOSS_8-YUKONSS_</t>
+  </si>
+  <si>
+    <t>FISHERRD_8-WCHTFLLS1_8 FLO BOWMAN_A-WFALLS_S</t>
+  </si>
+  <si>
+    <t>PECKTAP_9-SPRABERY_9 FLO BIGSPRIG-BIGSPRIG</t>
+  </si>
+  <si>
+    <t>COLETO4A-VICTORIA4A FLO COLETO4A-VICTORIA</t>
+  </si>
+  <si>
+    <t>VICTORIA4A-MAGRUDER4A FLO L_FPPYD1-L_FAYETT</t>
+  </si>
+  <si>
+    <t>DEERPK96T2_8-CARDIF_S96_8 FLO P_H_R_9-BAYOU__</t>
+  </si>
+  <si>
+    <t>RIOPECOS4A-TNWDWRDTAP1 FLO BASE</t>
+  </si>
+  <si>
+    <t>TNMAINLAND1-TNALVIN___1 FLO P_H_R__-MEADOW_</t>
+  </si>
+  <si>
+    <t>REDCREEK4A-BENFICKL4A FLO REDCREEK-COKESTRE</t>
+  </si>
+  <si>
+    <t>HAMILTON4B-MAXWELL4A FLO ILLN4A-L_FORTL</t>
+  </si>
+  <si>
+    <t>ESCONDID4A-EAGLE_PS4A FLO ESCONDID-EAGLE_PS</t>
+  </si>
+  <si>
+    <t>JEFFER_POI_8-S_CHAN_C06_8 FLO JEFFER_-COLEGE0</t>
+  </si>
+  <si>
+    <t>BRANCH 8283 8970 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 5901 80219 1</t>
+  </si>
+  <si>
+    <t>BRANCH 7104 7111 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 7104 7351 1</t>
+  </si>
+  <si>
+    <t>BRANCH 6341 6342 1</t>
   </si>
   <si>
     <t>BRANCHOPEN 6340 6360 1</t>
   </si>
   <si>
+    <t>BRANCH 3301 120162 1</t>
+  </si>
+  <si>
+    <t>BRANCH 6392 7130 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 6364 76390 1</t>
+  </si>
+  <si>
+    <t>BRANCH 221 2329 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 2241 2321 1</t>
+  </si>
+  <si>
     <t>BRANCH 8418 8961 1</t>
   </si>
   <si>
-    <t>BRANCHOPEN 8565 8961 1</t>
-  </si>
-  <si>
-    <t>BRANCH 6341 6342 1</t>
-  </si>
-  <si>
-    <t>BRANCH 3301 120162 1</t>
-  </si>
-  <si>
-    <t>BRANCH 6630 60385 1</t>
-  </si>
-  <si>
-    <t>BRANCHOPEN 60383 132331 1</t>
+    <t>BRANCHOPEN 8414 80470 1</t>
+  </si>
+  <si>
+    <t>BRANCH 1149 131853 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 1019 1250 2</t>
+  </si>
+  <si>
+    <t>BRANCH 1427 1448 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 1423 1464 1</t>
+  </si>
+  <si>
+    <t>BRANCH 1222 1330 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 1322 1323 1</t>
+  </si>
+  <si>
+    <t>BRANCH 8162 8172 2</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 8162 8172 1</t>
+  </si>
+  <si>
+    <t>BRANCH 8172 8194 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 7056 7057 1</t>
+  </si>
+  <si>
+    <t>BRANCH 40442 42240 96</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 42014 42160 96</t>
+  </si>
+  <si>
+    <t>BRANCH 6601 38330 1</t>
+  </si>
+  <si>
+    <t>BRANCH 38830 39030 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 42000 43030 99</t>
+  </si>
+  <si>
+    <t>BRANCH 6442 6473 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 6442 6449 1</t>
   </si>
   <si>
     <t>BRANCH 8257 8998 1</t>
   </si>
   <si>
-    <t>BRANCHOPEN 8283 78280 1</t>
-  </si>
-  <si>
-    <t>BRANCH 5799 80106 2</t>
-  </si>
-  <si>
-    <t>BRANCHOPEN 5799 80106 1</t>
-  </si>
-  <si>
-    <t>BRANCH 5915 42500 27</t>
-  </si>
-  <si>
-    <t>BRANCHOPEN 44000 44200 64</t>
-  </si>
-  <si>
-    <t>BRANCH 6666 6674 1</t>
-  </si>
-  <si>
-    <t>BRANCHOPEN 6628 6663 1</t>
-  </si>
-  <si>
-    <t>BRANCH 8516 85007 1</t>
-  </si>
-  <si>
-    <t>BRANCHOPEN 8458 8515 1</t>
-  </si>
-  <si>
-    <t>BRANCH 8255 8692 1</t>
-  </si>
-  <si>
-    <t>BRANCH 9079 9217 1</t>
-  </si>
-  <si>
-    <t>BRANCHOPEN 9045 9188 1</t>
+    <t>BRANCHOPEN 6564 76579 1</t>
+  </si>
+  <si>
+    <t>BRANCH 8260 8270 1</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 8260 8270 2</t>
+  </si>
+  <si>
+    <t>BRANCH 41240 41371 06</t>
+  </si>
+  <si>
+    <t>BRANCHOPEN 41240 42312 6</t>
   </si>
   <si>
     <t>NO</t>
   </si>
   <si>
-    <t>DHILMAR5</t>
-  </si>
-  <si>
-    <t>STEJGR38</t>
-  </si>
-  <si>
-    <t>SBRAUVA8</t>
+    <t>SLOBSA25</t>
+  </si>
+  <si>
+    <t>DFERSTA8</t>
   </si>
   <si>
     <t>SCOLBAL8</t>
   </si>
   <si>
-    <t>DHECWHI8</t>
-  </si>
-  <si>
     <t>BASE CASE</t>
   </si>
   <si>
-    <t>SWCSBOO8</t>
-  </si>
-  <si>
-    <t>SBEVASH8</t>
-  </si>
-  <si>
-    <t>SFALFAL8</t>
-  </si>
-  <si>
-    <t>DWAPHLJ5</t>
-  </si>
-  <si>
-    <t>SCOCBAR9</t>
-  </si>
-  <si>
-    <t>SALAN_28</t>
-  </si>
-  <si>
-    <t>DAUSDUN8</t>
-  </si>
-  <si>
-    <t>CIBOLO-SCHERT 138KV 293T304_1</t>
-  </si>
-  <si>
-    <t>CADDOTN-APACHE 138KV G138_4B_1</t>
-  </si>
-  <si>
-    <t>SONR-CTHR 138KV CTHR_SONR1_1</t>
-  </si>
-  <si>
-    <t>BALLINGE-HUMBLTAP 69KV BALLIN_HUMBLT1_1</t>
+    <t>SFORYEL8</t>
+  </si>
+  <si>
+    <t>SMGIENW8</t>
+  </si>
+  <si>
+    <t>SPORWH28</t>
+  </si>
+  <si>
+    <t>SECNMO28</t>
+  </si>
+  <si>
+    <t>DBOMLKW8</t>
+  </si>
+  <si>
+    <t>XBSP89</t>
+  </si>
+  <si>
+    <t>SVICCO28</t>
+  </si>
+  <si>
+    <t>DFPPFAY5</t>
+  </si>
+  <si>
+    <t>DPHRBBP8</t>
+  </si>
+  <si>
+    <t>MLOTYUC8</t>
+  </si>
+  <si>
+    <t>SMDOPHR5</t>
+  </si>
+  <si>
+    <t>SSACRED8</t>
+  </si>
+  <si>
+    <t>SILLFTL8</t>
+  </si>
+  <si>
+    <t>SEAGES28</t>
+  </si>
+  <si>
+    <t>DJFSCGR8</t>
+  </si>
+  <si>
+    <t>ASHERTON-CATARINA 138KV ASHERT_CATARI1_1</t>
+  </si>
+  <si>
+    <t>WIRTZ-FLATRO 138KV 38T365_1</t>
+  </si>
+  <si>
+    <t>HUMBLTAP-NOVICTAP 69KV HUMBLT_NOVICT1_1</t>
+  </si>
+  <si>
+    <t>GRDSW-NACPW 138KV NAC_L1_1</t>
+  </si>
+  <si>
+    <t>GILLES-FRPHILLT 69KV FRPHIL_GILLES1_1</t>
+  </si>
+  <si>
+    <t>ENSSW-TRU 138KV 921__D</t>
   </si>
   <si>
     <t>RINCON-WHITE_PT 138KV RINCON_WHITE_2_1</t>
   </si>
   <si>
-    <t>HUMBLTAP-NOVICTAP 69KV HUMBLT_NOVICT1_1</t>
-  </si>
-  <si>
-    <t>GRDSW-NACPW 138KV NAC_L1_1</t>
-  </si>
-  <si>
-    <t>FTST-SOLSTICE 138KV FTST_SOLSTI1_1</t>
+    <t>DHIDE-NOTSW 138KV 6100__F</t>
+  </si>
+  <si>
+    <t>FSHSW-WFALS 138KV 6558__B</t>
+  </si>
+  <si>
+    <t>SBYSW-PCKTP 69KV 6820__C</t>
+  </si>
+  <si>
+    <t>COLETO CREEK-VICTORIA 138KV COLETO_VICTOR2</t>
+  </si>
+  <si>
+    <t>VICTORIA-MAGRUDER 138KV MAGRUD_VICTOR2_1</t>
+  </si>
+  <si>
+    <t>DE-CA 138.10001KV CA_DE_96_A</t>
+  </si>
+  <si>
+    <t>RIOPECOS-WOODWRD2 138KV RIOPEC_WOODW21_1</t>
+  </si>
+  <si>
+    <t>ALVIN-MAINLAND 138KV 138_ALV_MNL_1</t>
+  </si>
+  <si>
+    <t>REDCREEK-BENFICKL 138KV BENFIC_REDCRE1_1</t>
   </si>
   <si>
     <t>MAXWELL-HAMILTON 138KV HAMILT_MAXWEL1_1</t>
   </si>
   <si>
-    <t>FALCNSW-FALCON 138KV FALCON_FALCNS2_1</t>
-  </si>
-  <si>
-    <t>STP-DOW 345KV DOWSTP27_A</t>
-  </si>
-  <si>
-    <t>BRONCO-ALPINE 69KV ALPINE_BRONCO1_1</t>
-  </si>
-  <si>
-    <t>N_SHARPE-CELANEBI 138KV CELANE_N_SHAR1_1</t>
-  </si>
-  <si>
-    <t>HAMILTON-MAVERICK 138KV HAMILT_MAVERI1_1</t>
-  </si>
-  <si>
-    <t>HWRDLN-MCNEIL 138KV CKT_972_1</t>
+    <t>ESCONDID-EAGLE_PS 138KV EAGLEP_ESCOND1_1</t>
+  </si>
+  <si>
+    <t>JFS-SC 138KV JFSSC_06_A</t>
   </si>
 </sst>
 </file>
@@ -602,7 +671,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -636,19 +705,19 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -659,19 +728,19 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -682,19 +751,19 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -705,19 +774,19 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="G5" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -728,19 +797,19 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -751,19 +820,19 @@
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="G7" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -774,19 +843,19 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="G8" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -794,22 +863,22 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="G9" t="s">
-        <v>65</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -820,19 +889,19 @@
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="G10" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -840,22 +909,22 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D11" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
-        <v>66</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -866,19 +935,19 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>52</v>
+        <v>67</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -886,22 +955,22 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="G13" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -912,19 +981,19 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -935,19 +1004,19 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -958,19 +1027,19 @@
         <v>13</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -981,19 +1050,19 @@
         <v>14</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D17" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1004,19 +1073,19 @@
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D18" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="G18" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1027,19 +1096,19 @@
         <v>15</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D19" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="G19" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1050,19 +1119,19 @@
         <v>15</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D20" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E20">
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1073,19 +1142,19 @@
         <v>16</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E21">
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="G21" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1096,19 +1165,19 @@
         <v>16</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E22">
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1119,19 +1188,19 @@
         <v>17</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="D23" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1142,19 +1211,19 @@
         <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E24">
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1165,19 +1234,19 @@
         <v>18</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E25">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="G25" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1188,19 +1257,19 @@
         <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="D26" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="G26" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1211,19 +1280,19 @@
         <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1231,22 +1300,22 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="G28" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1257,19 +1326,19 @@
         <v>20</v>
       </c>
       <c r="C29" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E29">
         <v>1</v>
       </c>
       <c r="F29" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="G29" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1277,22 +1346,183 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C30" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="E30">
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
       <c r="G30" t="s">
-        <v>76</v>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="D31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>77</v>
+      </c>
+      <c r="G31" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="1">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+      <c r="D33" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" t="s">
+        <v>57</v>
+      </c>
+      <c r="D34" t="s">
+        <v>61</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>79</v>
+      </c>
+      <c r="G34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" t="s">
+        <v>61</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>79</v>
+      </c>
+      <c r="G35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>80</v>
+      </c>
+      <c r="G36" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>80</v>
+      </c>
+      <c r="G37" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>